<commit_message>
Added IQR, Median, Mean to machine learning Cpx options following preprint.
</commit_message>
<xml_diff>
--- a/Examples/Cpx_Cpx_Liq_Thermobarometry/Cpx_Liquid_melt_matching/Gleeson2020JPET_Input_Pyroxene_Melts.xlsx
+++ b/Examples/Cpx_Cpx_Liq_Thermobarometry/Cpx_Liquid_melt_matching/Gleeson2020JPET_Input_Pyroxene_Melts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penny\OneDrive - University of Cambridge\Postdoc\PYthonBarometers\ClassicalThermometers-20210114T090546Z-001\ClassicalThermometers\Benchmarking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penny\OneDrive - Oregon State University\Postdoc\PyMME\MyBarometers\Thermobar_outer\Examples\Cpx_Cpx_Liq_Thermobarometry\Cpx_Liquid_melt_matching\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3A8E05-345D-4D8F-9A27-DA5B55B562F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1BA2ED-D173-4996-A977-D3A6E15AB632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{7CFCFF5C-2343-4223-9BFE-1F804DE7A7DC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{7CFCFF5C-2343-4223-9BFE-1F804DE7A7DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Cpxs" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="248">
   <si>
     <t>Na2O</t>
   </si>
@@ -790,13 +790,16 @@
     <t>core</t>
   </si>
   <si>
-    <t>Sample_ID</t>
-  </si>
-  <si>
     <t>FeOt_Liq</t>
   </si>
   <si>
     <t>FeOt_Cpx</t>
+  </si>
+  <si>
+    <t>Sample_ID_Liq</t>
+  </si>
+  <si>
+    <t>Sample_ID_Cpx</t>
   </si>
 </sst>
 </file>
@@ -2333,8 +2336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E5EC9DB-F635-43D6-9274-680C9C3F4410}">
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2344,7 +2347,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
@@ -2365,7 +2368,7 @@
         <v>15</v>
       </c>
       <c r="H1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I1" t="s">
         <v>16</v>
@@ -4880,8 +4883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28806BD5-E1D8-4405-9AED-F98C72058C18}">
   <dimension ref="A1:K164"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4891,7 +4894,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>32</v>
@@ -4918,7 +4921,7 @@
         <v>39</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>40</v>

</xml_diff>